<commit_message>
Nuevo muestreo de datos para la nueva vista del problema
</commit_message>
<xml_diff>
--- a/Doo-Doc/Nueva Version Victus/Modelo De Dominio Enriquecido Gestión de Residentes.xlsx
+++ b/Doo-Doc/Nueva Version Victus/Modelo De Dominio Enriquecido Gestión de Residentes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Documents\DOO 2024 BD\DOO\victus-doc\Doo-Doc\Nueva Version Victus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D387390-3C44-4C89-9D06-B678199F1132}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABFC273F-1EC1-4D7E-8700-159149DAF5CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="2" xr2:uid="{007C2ECE-7E90-4717-B1E7-3A143C146FF0}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{007C2ECE-7E90-4717-B1E7-3A143C146FF0}"/>
   </bookViews>
   <sheets>
     <sheet name="Valores" sheetId="1" r:id="rId1"/>
@@ -2424,8 +2424,8 @@
       <sheetName val="Publicación"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1" refreshError="1"/>
       <sheetData sheetId="2">
         <row r="3">
           <cell r="A3" t="str">
@@ -2444,12 +2444,12 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
+      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="5" refreshError="1"/>
+      <sheetData sheetId="6" refreshError="1"/>
+      <sheetData sheetId="7" refreshError="1"/>
+      <sheetData sheetId="8" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -2778,19 +2778,19 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="52.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="52.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="61" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="62"/>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -2798,7 +2798,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
@@ -2806,7 +2806,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>5</v>
       </c>
@@ -2814,52 +2814,52 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
         <v>15</v>
       </c>
@@ -2880,7 +2880,7 @@
       <selection activeCell="P34" sqref="P34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2891,20 +2891,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BB7FA3B-591F-4E21-A008-4E9729EA1949}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3:D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="56.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="11.42578125" style="8"/>
+    <col min="1" max="1" width="21.5546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="56.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="11.44140625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>16</v>
       </c>
@@ -2914,7 +2914,7 @@
       <c r="C1" s="63"/>
       <c r="D1" s="64"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
         <v>17</v>
       </c>
@@ -2928,7 +2928,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="12" t="s">
         <v>19</v>
       </c>
@@ -2943,7 +2943,7 @@
         <v>Residentes</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="12" t="s">
         <v>73</v>
       </c>
@@ -2956,7 +2956,7 @@
       </c>
       <c r="D4" s="66"/>
     </row>
-    <row r="5" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="12" t="s">
         <v>77</v>
       </c>
@@ -2986,38 +2986,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3CD2E3E-2179-4007-8743-BED3F3BF1317}">
   <dimension ref="A1:U25"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.5703125" style="8" customWidth="1"/>
-    <col min="3" max="3" width="18.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="28.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="61.28515625" style="8" customWidth="1"/>
-    <col min="10" max="10" width="79.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.5546875" style="8" customWidth="1"/>
+    <col min="3" max="3" width="18.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.5546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="61.33203125" style="8" customWidth="1"/>
+    <col min="10" max="10" width="79.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.44140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.88671875" style="8" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="25" style="8" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="94.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="132.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="46.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="50.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="66.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="52.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="23" max="16384" width="11.42578125" style="8"/>
+    <col min="17" max="17" width="94.44140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="132.5546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="46.44140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="50.109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="66.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="52.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="23" max="16384" width="11.44140625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" s="72" t="s">
         <v>20</v>
       </c>
@@ -3038,7 +3038,7 @@
       <c r="P1" s="72"/>
       <c r="Q1" s="72"/>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
         <v>21</v>
       </c>
@@ -3062,7 +3062,7 @@
       <c r="P2" s="73"/>
       <c r="Q2" s="73"/>
     </row>
-    <row r="3" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="15" t="s">
         <v>22</v>
       </c>
@@ -3086,7 +3086,7 @@
       <c r="P3" s="74"/>
       <c r="Q3" s="74"/>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4" s="16" t="s">
         <v>23</v>
       </c>
@@ -3155,7 +3155,7 @@
         <v>Reponsabilidad 4</v>
       </c>
     </row>
-    <row r="5" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A5" s="23" t="s">
         <v>39</v>
       </c>
@@ -3200,7 +3200,7 @@
       <c r="T5" s="30"/>
       <c r="U5" s="31"/>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A6" s="23" t="s">
         <v>44</v>
       </c>
@@ -3245,7 +3245,7 @@
       <c r="T6" s="30"/>
       <c r="U6" s="31"/>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A7" s="23" t="s">
         <v>79</v>
       </c>
@@ -3290,7 +3290,7 @@
       <c r="T7" s="30"/>
       <c r="U7" s="31"/>
     </row>
-    <row r="8" spans="1:21" ht="40.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A8" s="23" t="s">
         <v>81</v>
       </c>
@@ -3333,7 +3333,7 @@
       <c r="T8" s="30"/>
       <c r="U8" s="31"/>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A9" s="23" t="s">
         <v>82</v>
       </c>
@@ -3374,7 +3374,7 @@
       <c r="T9" s="30"/>
       <c r="U9" s="31"/>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A10" s="23" t="s">
         <v>83</v>
       </c>
@@ -3415,7 +3415,7 @@
       <c r="T10" s="30"/>
       <c r="U10" s="31"/>
     </row>
-    <row r="11" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A11" s="23" t="s">
         <v>72</v>
       </c>
@@ -3462,7 +3462,7 @@
       <c r="T11" s="30"/>
       <c r="U11" s="31"/>
     </row>
-    <row r="12" spans="1:21" ht="40.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A12" s="23" t="s">
         <v>84</v>
       </c>
@@ -3505,7 +3505,7 @@
       <c r="T12" s="30"/>
       <c r="U12" s="31"/>
     </row>
-    <row r="13" spans="1:21" ht="40.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A13" s="23" t="s">
         <v>80</v>
       </c>
@@ -3546,7 +3546,7 @@
       <c r="T13" s="30"/>
       <c r="U13" s="31"/>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A14" s="23" t="s">
         <v>74</v>
       </c>
@@ -3573,15 +3573,15 @@
       <c r="T14" s="30"/>
       <c r="U14" s="31"/>
     </row>
-    <row r="15" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A16" s="75" t="s">
         <v>51</v>
       </c>
       <c r="B16" s="76"/>
       <c r="C16" s="77"/>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A17" s="32" t="s">
         <v>52</v>
       </c>
@@ -3592,7 +3592,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="18" spans="1:19" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:19" ht="55.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="35" t="s">
         <v>54</v>
       </c>
@@ -3603,8 +3603,8 @@
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A20" s="78" t="s">
         <v>56</v>
       </c>
@@ -3637,7 +3637,7 @@
       </c>
       <c r="S20" s="82"/>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A21" s="80"/>
       <c r="B21" s="81"/>
       <c r="C21" s="81"/>
@@ -3676,7 +3676,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A22" s="83" t="s">
         <v>66</v>
       </c>
@@ -3699,7 +3699,7 @@
       <c r="R22" s="14"/>
       <c r="S22" s="40"/>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A23" s="68" t="s">
         <v>67</v>
       </c>
@@ -3722,7 +3722,7 @@
       <c r="R23" s="45"/>
       <c r="S23" s="46"/>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A24" s="86" t="s">
         <v>68</v>
       </c>
@@ -3745,7 +3745,7 @@
       <c r="R24" s="51"/>
       <c r="S24" s="52"/>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A25" s="90" t="s">
         <v>69</v>
       </c>
@@ -3834,34 +3834,34 @@
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.5703125" style="8" customWidth="1"/>
-    <col min="3" max="3" width="18.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="28.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="61.28515625" style="8" customWidth="1"/>
-    <col min="10" max="10" width="79.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.5546875" style="8" customWidth="1"/>
+    <col min="3" max="3" width="18.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.5546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="61.33203125" style="8" customWidth="1"/>
+    <col min="10" max="10" width="79.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.44140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.88671875" style="8" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="25" style="8" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="94.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="132.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="46.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="50.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="66.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="52.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="23" max="16384" width="11.42578125" style="8"/>
+    <col min="17" max="17" width="94.44140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="132.5546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="46.44140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="50.109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="66.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="52.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="23" max="16384" width="11.44140625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" s="72" t="s">
         <v>20</v>
       </c>
@@ -3882,7 +3882,7 @@
       <c r="P1" s="72"/>
       <c r="Q1" s="72"/>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
         <v>21</v>
       </c>
@@ -3906,7 +3906,7 @@
       <c r="P2" s="73"/>
       <c r="Q2" s="73"/>
     </row>
-    <row r="3" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="15" t="s">
         <v>22</v>
       </c>
@@ -3930,7 +3930,7 @@
       <c r="P3" s="74"/>
       <c r="Q3" s="74"/>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4" s="16" t="s">
         <v>23</v>
       </c>
@@ -3999,7 +3999,7 @@
         <v>Reponsabilidad 4</v>
       </c>
     </row>
-    <row r="5" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A5" s="23" t="s">
         <v>39</v>
       </c>
@@ -4044,7 +4044,7 @@
       <c r="T5" s="30"/>
       <c r="U5" s="31"/>
     </row>
-    <row r="6" spans="1:21" ht="54" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" ht="69" x14ac:dyDescent="0.3">
       <c r="A6" s="23" t="s">
         <v>44</v>
       </c>
@@ -4091,7 +4091,7 @@
       <c r="T6" s="30"/>
       <c r="U6" s="31"/>
     </row>
-    <row r="7" spans="1:21" ht="54" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" ht="69" x14ac:dyDescent="0.3">
       <c r="A7" s="23" t="s">
         <v>79</v>
       </c>
@@ -4138,7 +4138,7 @@
       <c r="T7" s="30"/>
       <c r="U7" s="31"/>
     </row>
-    <row r="8" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A8" s="23" t="s">
         <v>99</v>
       </c>
@@ -4185,7 +4185,7 @@
       <c r="T8" s="30"/>
       <c r="U8" s="31"/>
     </row>
-    <row r="9" spans="1:21" ht="40.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A9" s="23" t="s">
         <v>84</v>
       </c>
@@ -4228,7 +4228,7 @@
       <c r="T9" s="30"/>
       <c r="U9" s="31"/>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A10" s="23" t="s">
         <v>74</v>
       </c>
@@ -4255,17 +4255,17 @@
       <c r="T10" s="30"/>
       <c r="U10" s="31"/>
     </row>
-    <row r="11" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D11" s="59"/>
     </row>
-    <row r="12" spans="1:21" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="75" t="s">
         <v>51</v>
       </c>
       <c r="B12" s="76"/>
       <c r="C12" s="77"/>
     </row>
-    <row r="13" spans="1:21" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="32" t="s">
         <v>52</v>
       </c>
@@ -4276,7 +4276,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="14" spans="1:21" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:21" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="94" t="s">
         <v>101</v>
       </c>
@@ -4287,15 +4287,15 @@
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="1:21" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:21" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="95"/>
       <c r="B15" s="97"/>
       <c r="C15" s="37" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="16" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A17" s="78" t="s">
         <v>56</v>
       </c>
@@ -4328,7 +4328,7 @@
       </c>
       <c r="S17" s="82"/>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A18" s="80"/>
       <c r="B18" s="81"/>
       <c r="C18" s="81"/>
@@ -4367,7 +4367,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A19" s="83" t="s">
         <v>66</v>
       </c>
@@ -4390,7 +4390,7 @@
       <c r="R19" s="14"/>
       <c r="S19" s="40"/>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A20" s="68" t="s">
         <v>67</v>
       </c>
@@ -4413,7 +4413,7 @@
       <c r="R20" s="45"/>
       <c r="S20" s="46"/>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A21" s="86" t="s">
         <v>68</v>
       </c>
@@ -4436,7 +4436,7 @@
       <c r="R21" s="51"/>
       <c r="S21" s="52"/>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A22" s="90" t="s">
         <v>69</v>
       </c>
@@ -4516,34 +4516,34 @@
       <selection activeCell="A2" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.5703125" style="8" customWidth="1"/>
-    <col min="3" max="3" width="18.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="28.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="61.28515625" style="8" customWidth="1"/>
-    <col min="10" max="10" width="79.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.5546875" style="8" customWidth="1"/>
+    <col min="3" max="3" width="18.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.5546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="61.33203125" style="8" customWidth="1"/>
+    <col min="10" max="10" width="79.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.44140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.88671875" style="8" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="25" style="8" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="94.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="132.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="46.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="50.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="66.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="52.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="23" max="16384" width="11.42578125" style="8"/>
+    <col min="17" max="17" width="94.44140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="132.5546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="46.44140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="50.109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="66.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="52.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="23" max="16384" width="11.44140625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" s="72" t="s">
         <v>20</v>
       </c>
@@ -4564,7 +4564,7 @@
       <c r="P1" s="72"/>
       <c r="Q1" s="72"/>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
         <v>21</v>
       </c>
@@ -4588,7 +4588,7 @@
       <c r="P2" s="73"/>
       <c r="Q2" s="73"/>
     </row>
-    <row r="3" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="15" t="s">
         <v>22</v>
       </c>
@@ -4612,7 +4612,7 @@
       <c r="P3" s="74"/>
       <c r="Q3" s="74"/>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4" s="16" t="s">
         <v>23</v>
       </c>
@@ -4681,7 +4681,7 @@
         <v>Reponsabilidad 4</v>
       </c>
     </row>
-    <row r="5" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A5" s="23" t="s">
         <v>39</v>
       </c>
@@ -4726,7 +4726,7 @@
       <c r="T5" s="30"/>
       <c r="U5" s="31"/>
     </row>
-    <row r="6" spans="1:21" ht="54" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" ht="69" x14ac:dyDescent="0.3">
       <c r="A6" s="23" t="s">
         <v>44</v>
       </c>
@@ -4773,7 +4773,7 @@
       <c r="T6" s="30"/>
       <c r="U6" s="31"/>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A7" s="23" t="s">
         <v>103</v>
       </c>
@@ -4818,7 +4818,7 @@
       <c r="T7" s="30"/>
       <c r="U7" s="31"/>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A8" s="23" t="s">
         <v>84</v>
       </c>
@@ -4847,7 +4847,7 @@
       <c r="T8" s="30"/>
       <c r="U8" s="31"/>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A9" s="23" t="s">
         <v>107</v>
       </c>
@@ -4892,15 +4892,15 @@
       <c r="T9" s="30"/>
       <c r="U9" s="31"/>
     </row>
-    <row r="10" spans="1:21" ht="23.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="11" spans="1:21" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" ht="23.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="11" spans="1:21" ht="51" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="75" t="s">
         <v>51</v>
       </c>
       <c r="B11" s="76"/>
       <c r="C11" s="77"/>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A12" s="32" t="s">
         <v>52</v>
       </c>
@@ -4911,7 +4911,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="13" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="98" t="s">
         <v>109</v>
       </c>
@@ -4922,15 +4922,15 @@
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="99"/>
       <c r="B14" s="97"/>
       <c r="C14" s="60" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A16" s="78" t="s">
         <v>56</v>
       </c>
@@ -4963,7 +4963,7 @@
       </c>
       <c r="S16" s="82"/>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A17" s="80"/>
       <c r="B17" s="81"/>
       <c r="C17" s="81"/>
@@ -5002,7 +5002,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A18" s="83" t="s">
         <v>66</v>
       </c>
@@ -5025,7 +5025,7 @@
       <c r="R18" s="14"/>
       <c r="S18" s="40"/>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A19" s="68" t="s">
         <v>67</v>
       </c>
@@ -5048,7 +5048,7 @@
       <c r="R19" s="45"/>
       <c r="S19" s="46"/>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A20" s="86" t="s">
         <v>68</v>
       </c>
@@ -5071,7 +5071,7 @@
       <c r="R20" s="51"/>
       <c r="S20" s="52"/>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A21" s="90" t="s">
         <v>69</v>
       </c>

</xml_diff>